<commit_message>
creación de reporte HTML
</commit_message>
<xml_diff>
--- a/Diagrama de Gatt.xlsx
+++ b/Diagrama de Gatt.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\5to.BACHILLERATO\PRACTICA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\proyecto2022\practica2022NatalyAlvarez\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{899C50A3-55BB-4D53-BAD0-A91329D07C3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACFC981C-E47D-4500-9159-D55F8599FF8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{70482EC0-32A2-4E4F-95B6-32952FC475EF}"/>
   </bookViews>
@@ -367,9 +367,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -405,6 +402,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Énfasis6" xfId="1" builtinId="49"/>
@@ -1008,49 +1008,49 @@
       <c r="E2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="24" t="s">
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="N2" s="25"/>
-      <c r="O2" s="26"/>
+      <c r="N2" s="24"/>
+      <c r="O2" s="25"/>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C3" s="22"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="12" t="s">
+      <c r="C3" s="21"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="G3" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="H3" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="I3" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="J3" s="12" t="s">
+      <c r="J3" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="K3" s="12" t="s">
+      <c r="K3" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="L3" s="12" t="s">
+      <c r="L3" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="M3" s="17"/>
-      <c r="N3" s="11"/>
-      <c r="O3" s="18"/>
+      <c r="M3" s="16"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="17"/>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B4">
@@ -1065,18 +1065,18 @@
       <c r="E4" s="6">
         <v>44780</v>
       </c>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27" t="s">
+      <c r="F4" s="26"/>
+      <c r="G4" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="H4" s="27"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="17"/>
-      <c r="N4" s="11"/>
-      <c r="O4" s="18"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="17"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B5">
@@ -1091,15 +1091,15 @@
       <c r="E5" s="6">
         <v>44780</v>
       </c>
-      <c r="F5" s="16"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="28"/>
-      <c r="I5" s="28"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="13"/>
-      <c r="M5" s="17"/>
-      <c r="N5" s="11"/>
-      <c r="O5" s="18"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="27"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="12"/>
+      <c r="M5" s="16"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="17"/>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B6">
@@ -1114,15 +1114,15 @@
       <c r="E6" s="6">
         <v>44780</v>
       </c>
-      <c r="F6" s="16"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="13"/>
-      <c r="M6" s="17"/>
-      <c r="N6" s="11"/>
-      <c r="O6" s="18"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="12"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="10"/>
+      <c r="O6" s="17"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B7">
@@ -1137,14 +1137,14 @@
       <c r="E7" s="6">
         <v>44780</v>
       </c>
-      <c r="F7" s="16"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="29"/>
-      <c r="K7" s="13"/>
-      <c r="M7" s="17"/>
-      <c r="N7" s="11"/>
-      <c r="O7" s="18"/>
+      <c r="F7" s="15"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="28"/>
+      <c r="K7" s="12"/>
+      <c r="M7" s="16"/>
+      <c r="N7" s="10"/>
+      <c r="O7" s="17"/>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B8">
@@ -1159,14 +1159,14 @@
       <c r="E8" s="6">
         <v>44780</v>
       </c>
-      <c r="F8" s="16"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="14"/>
-      <c r="M8" s="19"/>
-      <c r="N8" s="20"/>
-      <c r="O8" s="21"/>
+      <c r="F8" s="15"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="13"/>
+      <c r="M8" s="18"/>
+      <c r="N8" s="19"/>
+      <c r="O8" s="20"/>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B9">
@@ -1181,15 +1181,15 @@
       <c r="E9" s="6">
         <v>44780</v>
       </c>
-      <c r="F9" s="15"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13"/>
-      <c r="K9" s="29"/>
-      <c r="L9" s="11"/>
-      <c r="M9" s="11"/>
-      <c r="N9" s="11"/>
-      <c r="O9" s="11"/>
+      <c r="F9" s="14"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="28"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="10"/>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B10">
@@ -1204,15 +1204,15 @@
       <c r="E10" s="6">
         <v>44780</v>
       </c>
-      <c r="F10" s="15"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="11"/>
-      <c r="M10" s="11"/>
-      <c r="N10" s="11"/>
-      <c r="O10" s="11"/>
+      <c r="F10" s="14"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="10"/>
+      <c r="O10" s="10"/>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B11">
@@ -1227,11 +1227,11 @@
       <c r="E11" s="6">
         <v>44780</v>
       </c>
-      <c r="F11" s="15"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="29"/>
+      <c r="F11" s="14"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="28"/>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B12">
@@ -1246,9 +1246,9 @@
       <c r="E12" s="6">
         <v>44787</v>
       </c>
-      <c r="F12" s="13"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="10"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="9"/>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B13">
@@ -1263,11 +1263,11 @@
       <c r="E13" s="6">
         <v>44787</v>
       </c>
-      <c r="F13" s="15"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="29"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="29"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="28"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="28"/>
       <c r="K13" s="7"/>
       <c r="L13" s="7"/>
     </row>
@@ -1284,11 +1284,11 @@
       <c r="E14" s="6">
         <v>44787</v>
       </c>
-      <c r="F14" s="15"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="13"/>
+      <c r="F14" s="14"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="12"/>
       <c r="L14" s="7"/>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">
@@ -1304,10 +1304,10 @@
       <c r="E15" s="6">
         <v>44787</v>
       </c>
-      <c r="F15" s="15"/>
-      <c r="J15" s="29"/>
-      <c r="K15" s="13"/>
-      <c r="L15" s="13"/>
+      <c r="F15" s="14"/>
+      <c r="J15" s="28"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="12"/>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B16">
@@ -1322,8 +1322,8 @@
       <c r="E16" s="6">
         <v>44792</v>
       </c>
-      <c r="F16" s="15"/>
-      <c r="H16" s="10"/>
+      <c r="F16" s="14"/>
+      <c r="H16" s="9"/>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B17">
@@ -1338,8 +1338,8 @@
       <c r="E17" s="6">
         <v>44792</v>
       </c>
-      <c r="F17" s="15"/>
-      <c r="J17" s="10"/>
+      <c r="F17" s="14"/>
+      <c r="J17" s="9"/>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B18">
@@ -1354,8 +1354,8 @@
       <c r="E18" s="6">
         <v>44792</v>
       </c>
-      <c r="F18" s="15"/>
-      <c r="J18" s="29"/>
+      <c r="F18" s="14"/>
+      <c r="J18" s="28"/>
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B19">
@@ -1370,12 +1370,12 @@
       <c r="E19" s="6">
         <v>44792</v>
       </c>
-      <c r="F19" s="15"/>
+      <c r="F19" s="14"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
-      <c r="J19" s="10"/>
-      <c r="K19" s="10"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B20">
@@ -1390,12 +1390,12 @@
       <c r="E20" s="6">
         <v>44799</v>
       </c>
-      <c r="F20" s="10"/>
+      <c r="F20" s="9"/>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
-      <c r="K20" s="13"/>
+      <c r="K20" s="12"/>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B21">
@@ -1410,8 +1410,8 @@
       <c r="E21" s="6">
         <v>44799</v>
       </c>
-      <c r="F21" s="13"/>
-      <c r="G21" s="29"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="28"/>
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
@@ -1430,8 +1430,8 @@
       <c r="E22" s="6">
         <v>44799</v>
       </c>
-      <c r="F22" s="15"/>
-      <c r="G22" s="10"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="9"/>
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
@@ -1450,9 +1450,9 @@
       <c r="E23" s="6">
         <v>44799</v>
       </c>
-      <c r="F23" s="15"/>
+      <c r="F23" s="14"/>
       <c r="G23" s="3"/>
-      <c r="H23" s="29"/>
+      <c r="H23" s="28"/>
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
@@ -1470,11 +1470,11 @@
       <c r="E24" s="6">
         <v>44799</v>
       </c>
-      <c r="F24" s="15"/>
+      <c r="F24" s="14"/>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
-      <c r="I24" s="13"/>
-      <c r="J24" s="10"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="9"/>
       <c r="K24" s="3"/>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.25">
@@ -1490,11 +1490,11 @@
       <c r="E25" s="6">
         <v>44799</v>
       </c>
-      <c r="F25" s="15"/>
+      <c r="F25" s="14"/>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
-      <c r="I25" s="13"/>
-      <c r="J25" s="29"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="28"/>
       <c r="K25" s="3"/>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.25">
@@ -1510,8 +1510,8 @@
       <c r="E26" s="6">
         <v>44806</v>
       </c>
-      <c r="F26" s="15"/>
-      <c r="G26" s="10"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="9"/>
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
@@ -1525,17 +1525,17 @@
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
-      <c r="G27" s="15"/>
+      <c r="G27" s="14"/>
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
-      <c r="M27" s="8" t="s">
+      <c r="M27" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="N27" s="8"/>
-      <c r="O27" s="8"/>
+      <c r="N27" s="29"/>
+      <c r="O27" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1550,8 +1550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{166A0605-256A-4EC0-BEB8-5543620DF797}">
   <dimension ref="B5:O30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1571,49 +1571,49 @@
       <c r="E5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="9"/>
-      <c r="M5" s="24" t="s">
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="N5" s="25"/>
-      <c r="O5" s="26"/>
+      <c r="N5" s="24"/>
+      <c r="O5" s="25"/>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C6" s="22"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="12" t="s">
+      <c r="C6" s="21"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="G6" s="12" t="s">
+      <c r="G6" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="H6" s="12" t="s">
+      <c r="H6" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="I6" s="12" t="s">
+      <c r="I6" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="J6" s="12" t="s">
+      <c r="J6" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="K6" s="12" t="s">
+      <c r="K6" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="L6" s="12" t="s">
+      <c r="L6" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="M6" s="17"/>
-      <c r="N6" s="11"/>
-      <c r="O6" s="18"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="10"/>
+      <c r="O6" s="17"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B7">
@@ -1628,18 +1628,18 @@
       <c r="E7" s="6">
         <v>44780</v>
       </c>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12" t="s">
+      <c r="F7" s="11"/>
+      <c r="G7" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="H7" s="27"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12"/>
-      <c r="M7" s="17"/>
-      <c r="N7" s="11"/>
-      <c r="O7" s="18"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="16"/>
+      <c r="N7" s="10"/>
+      <c r="O7" s="17"/>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B8">
@@ -1654,15 +1654,15 @@
       <c r="E8" s="6">
         <v>44780</v>
       </c>
-      <c r="F8" s="16"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="28"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="13"/>
-      <c r="M8" s="17"/>
-      <c r="N8" s="11"/>
-      <c r="O8" s="18"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="12"/>
+      <c r="M8" s="16"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="17"/>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B9">
@@ -1677,15 +1677,15 @@
       <c r="E9" s="6">
         <v>44780</v>
       </c>
-      <c r="F9" s="16"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
-      <c r="M9" s="17"/>
-      <c r="N9" s="11"/>
-      <c r="O9" s="18"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+      <c r="M9" s="16"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="17"/>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B10">
@@ -1700,14 +1700,14 @@
       <c r="E10" s="6">
         <v>44780</v>
       </c>
-      <c r="F10" s="16"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="29"/>
-      <c r="K10" s="13"/>
-      <c r="M10" s="17"/>
-      <c r="N10" s="11"/>
-      <c r="O10" s="18"/>
+      <c r="F10" s="15"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="28"/>
+      <c r="K10" s="12"/>
+      <c r="M10" s="16"/>
+      <c r="N10" s="10"/>
+      <c r="O10" s="17"/>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B11">
@@ -1722,14 +1722,14 @@
       <c r="E11" s="6">
         <v>44780</v>
       </c>
-      <c r="F11" s="16"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="14"/>
-      <c r="M11" s="19"/>
-      <c r="N11" s="20"/>
-      <c r="O11" s="21"/>
+      <c r="F11" s="15"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="13"/>
+      <c r="M11" s="18"/>
+      <c r="N11" s="19"/>
+      <c r="O11" s="20"/>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B12">
@@ -1744,15 +1744,15 @@
       <c r="E12" s="6">
         <v>44780</v>
       </c>
-      <c r="F12" s="15"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="29"/>
-      <c r="L12" s="11"/>
-      <c r="M12" s="11"/>
-      <c r="N12" s="11"/>
-      <c r="O12" s="11"/>
+      <c r="F12" s="14"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="28"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
+      <c r="N12" s="10"/>
+      <c r="O12" s="10"/>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B13">
@@ -1767,15 +1767,15 @@
       <c r="E13" s="6">
         <v>44780</v>
       </c>
-      <c r="F13" s="15"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="11"/>
-      <c r="M13" s="11"/>
-      <c r="N13" s="11"/>
-      <c r="O13" s="11"/>
+      <c r="F13" s="14"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="10"/>
+      <c r="O13" s="10"/>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B14">
@@ -1790,11 +1790,11 @@
       <c r="E14" s="6">
         <v>44780</v>
       </c>
-      <c r="F14" s="15"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="29"/>
+      <c r="F14" s="14"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="28"/>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B15">
@@ -1809,9 +1809,9 @@
       <c r="E15" s="6">
         <v>44787</v>
       </c>
-      <c r="F15" s="13"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="10"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="9"/>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B16">
@@ -1826,11 +1826,11 @@
       <c r="E16" s="6">
         <v>44787</v>
       </c>
-      <c r="F16" s="15"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="29"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="29"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="28"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="28"/>
       <c r="K16" s="7"/>
       <c r="L16" s="7"/>
     </row>
@@ -1847,11 +1847,11 @@
       <c r="E17" s="6">
         <v>44787</v>
       </c>
-      <c r="F17" s="15"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="10"/>
-      <c r="K17" s="13"/>
+      <c r="F17" s="14"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="12"/>
       <c r="L17" s="7"/>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.25">
@@ -1867,10 +1867,10 @@
       <c r="E18" s="6">
         <v>44787</v>
       </c>
-      <c r="F18" s="15"/>
-      <c r="J18" s="29"/>
-      <c r="K18" s="13"/>
-      <c r="L18" s="13"/>
+      <c r="F18" s="14"/>
+      <c r="J18" s="28"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="12"/>
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B19">
@@ -1885,8 +1885,8 @@
       <c r="E19" s="6">
         <v>44792</v>
       </c>
-      <c r="F19" s="15"/>
-      <c r="H19" s="10"/>
+      <c r="F19" s="14"/>
+      <c r="H19" s="9"/>
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B20">
@@ -1901,8 +1901,8 @@
       <c r="E20" s="6">
         <v>44792</v>
       </c>
-      <c r="F20" s="15"/>
-      <c r="J20" s="10"/>
+      <c r="F20" s="14"/>
+      <c r="J20" s="9"/>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B21">
@@ -1917,8 +1917,8 @@
       <c r="E21" s="6">
         <v>44792</v>
       </c>
-      <c r="F21" s="15"/>
-      <c r="J21" s="29"/>
+      <c r="F21" s="14"/>
+      <c r="J21" s="28"/>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B22">
@@ -1933,12 +1933,12 @@
       <c r="E22" s="6">
         <v>44792</v>
       </c>
-      <c r="F22" s="15"/>
+      <c r="F22" s="14"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
-      <c r="J22" s="10"/>
-      <c r="K22" s="10"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B23">
@@ -1953,12 +1953,12 @@
       <c r="E23" s="6">
         <v>44799</v>
       </c>
-      <c r="F23" s="10"/>
+      <c r="F23" s="9"/>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
-      <c r="K23" s="13"/>
+      <c r="K23" s="12"/>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B24">
@@ -1973,8 +1973,8 @@
       <c r="E24" s="6">
         <v>44799</v>
       </c>
-      <c r="F24" s="13"/>
-      <c r="G24" s="29"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="28"/>
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
@@ -1993,8 +1993,8 @@
       <c r="E25" s="6">
         <v>44799</v>
       </c>
-      <c r="F25" s="15"/>
-      <c r="G25" s="10"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="9"/>
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
@@ -2008,14 +2008,14 @@
         <v>22</v>
       </c>
       <c r="D26" s="6">
-        <v>44798</v>
+        <v>44802</v>
       </c>
       <c r="E26" s="6">
-        <v>44799</v>
-      </c>
-      <c r="F26" s="15"/>
+        <v>44806</v>
+      </c>
+      <c r="F26" s="14"/>
       <c r="G26" s="3"/>
-      <c r="H26" s="29"/>
+      <c r="H26" s="28"/>
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
@@ -2028,16 +2028,16 @@
         <v>23</v>
       </c>
       <c r="D27" s="6">
-        <v>44799</v>
+        <v>44802</v>
       </c>
       <c r="E27" s="6">
-        <v>44799</v>
-      </c>
-      <c r="F27" s="15"/>
+        <v>44806</v>
+      </c>
+      <c r="F27" s="14"/>
       <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
-      <c r="I27" s="13"/>
-      <c r="J27" s="10"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="12"/>
       <c r="K27" s="3"/>
     </row>
     <row r="28" spans="2:15" x14ac:dyDescent="0.25">
@@ -2048,16 +2048,16 @@
         <v>24</v>
       </c>
       <c r="D28" s="6">
-        <v>44799</v>
+        <v>44802</v>
       </c>
       <c r="E28" s="6">
-        <v>44799</v>
-      </c>
-      <c r="F28" s="15"/>
+        <v>44806</v>
+      </c>
+      <c r="F28" s="14"/>
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
-      <c r="I28" s="13"/>
-      <c r="J28" s="29"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="12"/>
       <c r="K28" s="3"/>
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.25">
@@ -2073,8 +2073,8 @@
       <c r="E29" s="6">
         <v>44806</v>
       </c>
-      <c r="F29" s="15"/>
-      <c r="G29" s="10"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="12"/>
       <c r="H29" s="3"/>
       <c r="I29" s="3"/>
       <c r="J29" s="3"/>
@@ -2088,17 +2088,17 @@
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
       <c r="F30" s="6"/>
-      <c r="G30" s="15"/>
+      <c r="G30" s="14"/>
       <c r="H30" s="3"/>
       <c r="I30" s="3"/>
       <c r="J30" s="3"/>
       <c r="K30" s="3"/>
       <c r="L30" s="3"/>
-      <c r="M30" s="8" t="s">
+      <c r="M30" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="N30" s="8"/>
-      <c r="O30" s="8"/>
+      <c r="N30" s="29"/>
+      <c r="O30" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
edición de botones y orden de burbuja clientes y creación de visión productos
</commit_message>
<xml_diff>
--- a/Diagrama de Gatt.xlsx
+++ b/Diagrama de Gatt.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\proyecto2022\practica2022NatalyAlvarez\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACFC981C-E47D-4500-9159-D55F8599FF8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{382F84DF-D640-4830-BF17-8FE35A942D4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{70482EC0-32A2-4E4F-95B6-32952FC475EF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{70482EC0-32A2-4E4F-95B6-32952FC475EF}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>Nombre de Actividad</t>
   </si>
@@ -145,6 +144,9 @@
   </si>
   <si>
     <t>Dom.</t>
+  </si>
+  <si>
+    <t>Crear tabla para visualizar productos</t>
   </si>
 </sst>
 </file>
@@ -438,92 +440,6 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>57149</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>85724</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="2047875" cy="962025"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Imagen 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53C26338-A4ED-42C0-A606-C0EBE6857F42}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:srcRect l="2992" t="21982" r="5127" b="6396"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11439524" y="466724"/>
-          <a:ext cx="2047875" cy="962025"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>9861</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>57283</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Imagen 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{471BC724-4970-6EA8-6463-1C3323FC4898}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:srcRect l="2371"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11325225" y="5200650"/>
-          <a:ext cx="2353011" cy="952633"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
@@ -981,577 +897,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F80FD00-3111-4D0A-A82A-8807C83A5F2D}">
-  <dimension ref="B2:O27"/>
-  <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:O33"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.5703125" customWidth="1"/>
-    <col min="2" max="2" width="4.42578125" customWidth="1"/>
-    <col min="3" max="3" width="82.28515625" customWidth="1"/>
-    <col min="4" max="5" width="15.42578125" customWidth="1"/>
-    <col min="6" max="11" width="5" customWidth="1"/>
-    <col min="12" max="12" width="5.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="N2" s="24"/>
-      <c r="O2" s="25"/>
-    </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C3" s="21"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="G3" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="H3" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="I3" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="J3" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="K3" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="L3" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="M3" s="16"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="17"/>
-    </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="6">
-        <v>44774</v>
-      </c>
-      <c r="E4" s="6">
-        <v>44780</v>
-      </c>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26" t="s">
-        <v>29</v>
-      </c>
-      <c r="H4" s="26"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="16"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="17"/>
-    </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="6">
-        <v>44775</v>
-      </c>
-      <c r="E5" s="6">
-        <v>44780</v>
-      </c>
-      <c r="F5" s="15"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="27"/>
-      <c r="I5" s="27"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="12"/>
-      <c r="M5" s="16"/>
-      <c r="N5" s="10"/>
-      <c r="O5" s="17"/>
-    </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B6">
-        <v>3</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="6">
-        <v>44775</v>
-      </c>
-      <c r="E6" s="6">
-        <v>44780</v>
-      </c>
-      <c r="F6" s="15"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="12"/>
-      <c r="M6" s="16"/>
-      <c r="N6" s="10"/>
-      <c r="O6" s="17"/>
-    </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B7">
-        <v>4</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="6">
-        <v>44776</v>
-      </c>
-      <c r="E7" s="6">
-        <v>44780</v>
-      </c>
-      <c r="F7" s="15"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="28"/>
-      <c r="K7" s="12"/>
-      <c r="M7" s="16"/>
-      <c r="N7" s="10"/>
-      <c r="O7" s="17"/>
-    </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B8">
-        <v>5</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="6">
-        <v>44777</v>
-      </c>
-      <c r="E8" s="6">
-        <v>44780</v>
-      </c>
-      <c r="F8" s="15"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="13"/>
-      <c r="M8" s="18"/>
-      <c r="N8" s="19"/>
-      <c r="O8" s="20"/>
-    </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B9">
-        <v>6</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="6">
-        <v>44778</v>
-      </c>
-      <c r="E9" s="6">
-        <v>44780</v>
-      </c>
-      <c r="F9" s="14"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="28"/>
-      <c r="L9" s="10"/>
-      <c r="M9" s="10"/>
-      <c r="N9" s="10"/>
-      <c r="O9" s="10"/>
-    </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B10">
-        <v>7</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="6">
-        <v>44778</v>
-      </c>
-      <c r="E10" s="6">
-        <v>44780</v>
-      </c>
-      <c r="F10" s="14"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="10"/>
-      <c r="M10" s="10"/>
-      <c r="N10" s="10"/>
-      <c r="O10" s="10"/>
-    </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B11">
-        <v>8</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="6">
-        <v>44778</v>
-      </c>
-      <c r="E11" s="6">
-        <v>44780</v>
-      </c>
-      <c r="F11" s="14"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="28"/>
-    </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B12">
-        <v>9</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="6">
-        <v>44781</v>
-      </c>
-      <c r="E12" s="6">
-        <v>44787</v>
-      </c>
-      <c r="F12" s="12"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="9"/>
-    </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B13">
-        <v>10</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" s="6">
-        <v>44782</v>
-      </c>
-      <c r="E13" s="6">
-        <v>44787</v>
-      </c>
-      <c r="F13" s="14"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="28"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="28"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7"/>
-    </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B14">
-        <v>11</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" s="6">
-        <v>44782</v>
-      </c>
-      <c r="E14" s="6">
-        <v>44787</v>
-      </c>
-      <c r="F14" s="14"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="9"/>
-      <c r="K14" s="12"/>
-      <c r="L14" s="7"/>
-    </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B15">
-        <v>12</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D15" s="6">
-        <v>44783</v>
-      </c>
-      <c r="E15" s="6">
-        <v>44787</v>
-      </c>
-      <c r="F15" s="14"/>
-      <c r="J15" s="28"/>
-      <c r="K15" s="12"/>
-      <c r="L15" s="12"/>
-    </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B16">
-        <v>13</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D16" s="6">
-        <v>44789</v>
-      </c>
-      <c r="E16" s="6">
-        <v>44792</v>
-      </c>
-      <c r="F16" s="14"/>
-      <c r="H16" s="9"/>
-    </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B17">
-        <v>14</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D17" s="6">
-        <v>44791</v>
-      </c>
-      <c r="E17" s="6">
-        <v>44792</v>
-      </c>
-      <c r="F17" s="14"/>
-      <c r="J17" s="9"/>
-    </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B18">
-        <v>15</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D18" s="6">
-        <v>44791</v>
-      </c>
-      <c r="E18" s="6">
-        <v>44792</v>
-      </c>
-      <c r="F18" s="14"/>
-      <c r="J18" s="28"/>
-    </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B19">
-        <v>16</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D19" s="6">
-        <v>44792</v>
-      </c>
-      <c r="E19" s="6">
-        <v>44792</v>
-      </c>
-      <c r="F19" s="14"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="9"/>
-      <c r="K19" s="9"/>
-    </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B20">
-        <v>17</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D20" s="6">
-        <v>44795</v>
-      </c>
-      <c r="E20" s="6">
-        <v>44799</v>
-      </c>
-      <c r="F20" s="9"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="12"/>
-    </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B21">
-        <v>18</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D21" s="6">
-        <v>44797</v>
-      </c>
-      <c r="E21" s="6">
-        <v>44799</v>
-      </c>
-      <c r="F21" s="12"/>
-      <c r="G21" s="28"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
-    </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B22">
-        <v>19</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D22" s="6">
-        <v>44798</v>
-      </c>
-      <c r="E22" s="6">
-        <v>44799</v>
-      </c>
-      <c r="F22" s="14"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="3"/>
-    </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B23">
-        <v>20</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D23" s="6">
-        <v>44798</v>
-      </c>
-      <c r="E23" s="6">
-        <v>44799</v>
-      </c>
-      <c r="F23" s="14"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="28"/>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
-      <c r="K23" s="3"/>
-    </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B24">
-        <v>21</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D24" s="6">
-        <v>44799</v>
-      </c>
-      <c r="E24" s="6">
-        <v>44799</v>
-      </c>
-      <c r="F24" s="14"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="12"/>
-      <c r="J24" s="9"/>
-      <c r="K24" s="3"/>
-    </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B25">
-        <v>22</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D25" s="6">
-        <v>44799</v>
-      </c>
-      <c r="E25" s="6">
-        <v>44799</v>
-      </c>
-      <c r="F25" s="14"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="12"/>
-      <c r="J25" s="28"/>
-      <c r="K25" s="3"/>
-    </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B26">
-        <v>23</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D26" s="6">
-        <v>44802</v>
-      </c>
-      <c r="E26" s="6">
-        <v>44806</v>
-      </c>
-      <c r="F26" s="14"/>
-      <c r="G26" s="9"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
-      <c r="K26" s="3"/>
-    </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B27">
-        <v>24</v>
-      </c>
-      <c r="C27" s="1"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="3"/>
-      <c r="I27" s="3"/>
-      <c r="J27" s="3"/>
-      <c r="K27" s="3"/>
-      <c r="L27" s="3"/>
-      <c r="M27" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="N27" s="29"/>
-      <c r="O27" s="29"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="M27:O27"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{166A0605-256A-4EC0-BEB8-5543620DF797}">
   <dimension ref="B5:O30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2056,7 +1406,7 @@
       <c r="F28" s="14"/>
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
-      <c r="I28" s="12"/>
+      <c r="I28" s="28"/>
       <c r="J28" s="12"/>
       <c r="K28" s="3"/>
     </row>
@@ -2077,16 +1427,22 @@
       <c r="G29" s="12"/>
       <c r="H29" s="3"/>
       <c r="I29" s="3"/>
-      <c r="J29" s="3"/>
+      <c r="J29" s="9"/>
       <c r="K29" s="3"/>
     </row>
     <row r="30" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B30">
         <v>24</v>
       </c>
-      <c r="C30" s="1"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
+      <c r="C30" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D30" s="6">
+        <v>44805</v>
+      </c>
+      <c r="E30" s="6">
+        <v>44806</v>
+      </c>
       <c r="F30" s="6"/>
       <c r="G30" s="14"/>
       <c r="H30" s="3"/>
@@ -2105,6 +1461,7 @@
     <mergeCell ref="M30:O30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
creación de la tabla productos, visualización de ejemplos de productos y partes del archivo CSV
</commit_message>
<xml_diff>
--- a/Diagrama de Gatt.xlsx
+++ b/Diagrama de Gatt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\proyecto2022\practica2022NatalyAlvarez\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{382F84DF-D640-4830-BF17-8FE35A942D4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BEDCF07-8A3E-4746-87C5-49D4675E58EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{70482EC0-32A2-4E4F-95B6-32952FC475EF}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
   <si>
     <t>Nombre de Actividad</t>
   </si>
@@ -147,6 +147,9 @@
   </si>
   <si>
     <t>Crear tabla para visualizar productos</t>
+  </si>
+  <si>
+    <t>Leer productos de prueba para mostrar en la tabla</t>
   </si>
 </sst>
 </file>
@@ -358,7 +361,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -368,19 +371,15 @@
     <xf numFmtId="16" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -397,16 +396,17 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Énfasis6" xfId="1" builtinId="49"/>
@@ -898,10 +898,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{166A0605-256A-4EC0-BEB8-5543620DF797}">
-  <dimension ref="B5:O30"/>
+  <dimension ref="B5:O36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -921,49 +921,48 @@
       <c r="E5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="23" t="s">
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="N5" s="24"/>
-      <c r="O5" s="25"/>
+      <c r="N5" s="20"/>
+      <c r="O5" s="21"/>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C6" s="21"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="11" t="s">
+      <c r="C6" s="17"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="G6" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="H6" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="I6" s="11" t="s">
+      <c r="I6" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="J6" s="11" t="s">
+      <c r="J6" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="K6" s="11" t="s">
+      <c r="K6" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="L6" s="11" t="s">
+      <c r="L6" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="M6" s="16"/>
-      <c r="N6" s="10"/>
-      <c r="O6" s="17"/>
+      <c r="M6" s="12"/>
+      <c r="O6" s="13"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B7">
@@ -978,18 +977,17 @@
       <c r="E7" s="6">
         <v>44780</v>
       </c>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11" t="s">
+      <c r="F7" s="9"/>
+      <c r="G7" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="H7" s="26"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="11"/>
-      <c r="L7" s="11"/>
-      <c r="M7" s="16"/>
-      <c r="N7" s="10"/>
-      <c r="O7" s="17"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="12"/>
+      <c r="O7" s="13"/>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B8">
@@ -1004,15 +1002,11 @@
       <c r="E8" s="6">
         <v>44780</v>
       </c>
-      <c r="F8" s="15"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="27"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="12"/>
-      <c r="M8" s="16"/>
-      <c r="N8" s="10"/>
-      <c r="O8" s="17"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="M8" s="12"/>
+      <c r="O8" s="13"/>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B9">
@@ -1027,15 +1021,9 @@
       <c r="E9" s="6">
         <v>44780</v>
       </c>
-      <c r="F9" s="15"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="12"/>
-      <c r="M9" s="16"/>
-      <c r="N9" s="10"/>
-      <c r="O9" s="17"/>
+      <c r="I9" s="8"/>
+      <c r="M9" s="12"/>
+      <c r="O9" s="13"/>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B10">
@@ -1050,14 +1038,9 @@
       <c r="E10" s="6">
         <v>44780</v>
       </c>
-      <c r="F10" s="15"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="28"/>
-      <c r="K10" s="12"/>
-      <c r="M10" s="16"/>
-      <c r="N10" s="10"/>
-      <c r="O10" s="17"/>
+      <c r="J10" s="24"/>
+      <c r="M10" s="12"/>
+      <c r="O10" s="13"/>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B11">
@@ -1072,14 +1055,11 @@
       <c r="E11" s="6">
         <v>44780</v>
       </c>
-      <c r="F11" s="15"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="13"/>
-      <c r="M11" s="18"/>
-      <c r="N11" s="19"/>
-      <c r="O11" s="20"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="10"/>
+      <c r="M11" s="14"/>
+      <c r="N11" s="15"/>
+      <c r="O11" s="16"/>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B12">
@@ -1094,15 +1074,8 @@
       <c r="E12" s="6">
         <v>44780</v>
       </c>
-      <c r="F12" s="14"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="28"/>
-      <c r="L12" s="10"/>
-      <c r="M12" s="10"/>
-      <c r="N12" s="10"/>
-      <c r="O12" s="10"/>
+      <c r="F12" s="11"/>
+      <c r="K12" s="24"/>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B13">
@@ -1117,15 +1090,8 @@
       <c r="E13" s="6">
         <v>44780</v>
       </c>
-      <c r="F13" s="14"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="10"/>
-      <c r="M13" s="10"/>
-      <c r="N13" s="10"/>
-      <c r="O13" s="10"/>
+      <c r="F13" s="11"/>
+      <c r="K13" s="8"/>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B14">
@@ -1140,11 +1106,8 @@
       <c r="E14" s="6">
         <v>44780</v>
       </c>
-      <c r="F14" s="14"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="28"/>
+      <c r="F14" s="11"/>
+      <c r="K14" s="24"/>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B15">
@@ -1159,9 +1122,8 @@
       <c r="E15" s="6">
         <v>44787</v>
       </c>
-      <c r="F15" s="12"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="9"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="8"/>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B16">
@@ -1176,13 +1138,9 @@
       <c r="E16" s="6">
         <v>44787</v>
       </c>
-      <c r="F16" s="14"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="28"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="28"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
+      <c r="F16" s="11"/>
+      <c r="H16" s="24"/>
+      <c r="J16" s="24"/>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B17">
@@ -1197,12 +1155,9 @@
       <c r="E17" s="6">
         <v>44787</v>
       </c>
-      <c r="F17" s="14"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="9"/>
-      <c r="K17" s="12"/>
-      <c r="L17" s="7"/>
+      <c r="F17" s="11"/>
+      <c r="H17" s="8"/>
+      <c r="J17" s="8"/>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B18">
@@ -1217,10 +1172,8 @@
       <c r="E18" s="6">
         <v>44787</v>
       </c>
-      <c r="F18" s="14"/>
-      <c r="J18" s="28"/>
-      <c r="K18" s="12"/>
-      <c r="L18" s="12"/>
+      <c r="F18" s="11"/>
+      <c r="J18" s="24"/>
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B19">
@@ -1235,8 +1188,8 @@
       <c r="E19" s="6">
         <v>44792</v>
       </c>
-      <c r="F19" s="14"/>
-      <c r="H19" s="9"/>
+      <c r="F19" s="11"/>
+      <c r="H19" s="8"/>
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B20">
@@ -1251,8 +1204,8 @@
       <c r="E20" s="6">
         <v>44792</v>
       </c>
-      <c r="F20" s="14"/>
-      <c r="J20" s="9"/>
+      <c r="F20" s="11"/>
+      <c r="J20" s="8"/>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B21">
@@ -1267,8 +1220,8 @@
       <c r="E21" s="6">
         <v>44792</v>
       </c>
-      <c r="F21" s="14"/>
-      <c r="J21" s="28"/>
+      <c r="F21" s="11"/>
+      <c r="J21" s="24"/>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B22">
@@ -1283,12 +1236,12 @@
       <c r="E22" s="6">
         <v>44792</v>
       </c>
-      <c r="F22" s="14"/>
+      <c r="F22" s="11"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
-      <c r="J22" s="9"/>
-      <c r="K22" s="9"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B23">
@@ -1303,12 +1256,11 @@
       <c r="E23" s="6">
         <v>44799</v>
       </c>
-      <c r="F23" s="9"/>
+      <c r="F23" s="8"/>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
-      <c r="K23" s="12"/>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B24">
@@ -1323,8 +1275,7 @@
       <c r="E24" s="6">
         <v>44799</v>
       </c>
-      <c r="F24" s="12"/>
-      <c r="G24" s="28"/>
+      <c r="G24" s="24"/>
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
@@ -1343,8 +1294,8 @@
       <c r="E25" s="6">
         <v>44799</v>
       </c>
-      <c r="F25" s="14"/>
-      <c r="G25" s="9"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="8"/>
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
@@ -1363,9 +1314,9 @@
       <c r="E26" s="6">
         <v>44806</v>
       </c>
-      <c r="F26" s="14"/>
+      <c r="F26" s="11"/>
       <c r="G26" s="3"/>
-      <c r="H26" s="28"/>
+      <c r="H26" s="24"/>
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
@@ -1383,11 +1334,9 @@
       <c r="E27" s="6">
         <v>44806</v>
       </c>
-      <c r="F27" s="14"/>
+      <c r="F27" s="11"/>
       <c r="G27" s="3"/>
-      <c r="H27" s="9"/>
-      <c r="I27" s="12"/>
-      <c r="J27" s="12"/>
+      <c r="H27" s="8"/>
       <c r="K27" s="3"/>
     </row>
     <row r="28" spans="2:15" x14ac:dyDescent="0.25">
@@ -1403,11 +1352,11 @@
       <c r="E28" s="6">
         <v>44806</v>
       </c>
-      <c r="F28" s="14"/>
+      <c r="F28" s="11"/>
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
-      <c r="I28" s="28"/>
-      <c r="J28" s="12"/>
+      <c r="I28" s="24"/>
+      <c r="J28" s="26"/>
       <c r="K28" s="3"/>
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.25">
@@ -1423,11 +1372,10 @@
       <c r="E29" s="6">
         <v>44806</v>
       </c>
-      <c r="F29" s="14"/>
-      <c r="G29" s="12"/>
+      <c r="F29" s="11"/>
       <c r="H29" s="3"/>
-      <c r="I29" s="3"/>
-      <c r="J29" s="9"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="26"/>
       <c r="K29" s="3"/>
     </row>
     <row r="30" spans="2:15" x14ac:dyDescent="0.25">
@@ -1444,17 +1392,67 @@
         <v>44806</v>
       </c>
       <c r="F30" s="6"/>
-      <c r="G30" s="14"/>
+      <c r="G30" s="11"/>
       <c r="H30" s="3"/>
-      <c r="I30" s="3"/>
-      <c r="J30" s="3"/>
+      <c r="I30" s="24"/>
+      <c r="J30" s="26"/>
       <c r="K30" s="3"/>
       <c r="L30" s="3"/>
-      <c r="M30" s="29" t="s">
+      <c r="M30" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="N30" s="29"/>
-      <c r="O30" s="29"/>
+      <c r="N30" s="25"/>
+      <c r="O30" s="25"/>
+    </row>
+    <row r="31" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <v>25</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D31" s="6">
+        <v>44805</v>
+      </c>
+      <c r="E31" s="6">
+        <v>44806</v>
+      </c>
+      <c r="I31" s="8"/>
+    </row>
+    <row r="32" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <v>26</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D32" s="6">
+        <v>44805</v>
+      </c>
+      <c r="E32" s="6">
+        <v>44806</v>
+      </c>
+      <c r="I32" s="24"/>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B35">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B36">
+        <v>30</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
creación de grafica de barras, botones de CSV,HTML y volver,ERROR EN EL HTML
</commit_message>
<xml_diff>
--- a/Diagrama de Gatt.xlsx
+++ b/Diagrama de Gatt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\proyecto2022\practica2022NatalyAlvarez\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BEDCF07-8A3E-4746-87C5-49D4675E58EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B835C444-3050-418A-B699-3EF1DDA89656}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{70482EC0-32A2-4E4F-95B6-32952FC475EF}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="40">
   <si>
     <t>Nombre de Actividad</t>
   </si>
@@ -150,6 +150,9 @@
   </si>
   <si>
     <t>Leer productos de prueba para mostrar en la tabla</t>
+  </si>
+  <si>
+    <t>Edición final de botones y orden burbuja para productos</t>
   </si>
 </sst>
 </file>
@@ -361,7 +364,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -406,6 +409,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -898,10 +902,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{166A0605-256A-4EC0-BEB8-5543620DF797}">
-  <dimension ref="B5:O36"/>
+  <dimension ref="B5:O42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="B3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1356,7 +1360,6 @@
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
       <c r="I28" s="24"/>
-      <c r="J28" s="26"/>
       <c r="K28" s="3"/>
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.25">
@@ -1375,7 +1378,6 @@
       <c r="F29" s="11"/>
       <c r="H29" s="3"/>
       <c r="I29" s="8"/>
-      <c r="J29" s="26"/>
       <c r="K29" s="3"/>
     </row>
     <row r="30" spans="2:15" x14ac:dyDescent="0.25">
@@ -1395,7 +1397,6 @@
       <c r="G30" s="11"/>
       <c r="H30" s="3"/>
       <c r="I30" s="24"/>
-      <c r="J30" s="26"/>
       <c r="K30" s="3"/>
       <c r="L30" s="3"/>
       <c r="M30" s="25" t="s">
@@ -1434,25 +1435,131 @@
       </c>
       <c r="I32" s="24"/>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B33">
         <v>27</v>
       </c>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C33" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D33" s="6">
+        <v>44805</v>
+      </c>
+      <c r="E33" s="6">
+        <v>44806</v>
+      </c>
+      <c r="I33" s="8"/>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34">
         <v>28</v>
       </c>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C34" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D34" s="6">
+        <v>44805</v>
+      </c>
+      <c r="E34" s="6">
+        <v>44806</v>
+      </c>
+      <c r="I34" s="24"/>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35">
         <v>29</v>
       </c>
-    </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C35" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D35" s="6">
+        <v>44805</v>
+      </c>
+      <c r="E35" s="6">
+        <v>44806</v>
+      </c>
+      <c r="I35" s="24"/>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36">
         <v>30</v>
       </c>
+      <c r="C36" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D36" s="6">
+        <v>44805</v>
+      </c>
+      <c r="E36" s="6">
+        <v>44806</v>
+      </c>
+      <c r="I36" s="8"/>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B37">
+        <v>31</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D37" s="6">
+        <v>44805</v>
+      </c>
+      <c r="E37" s="6">
+        <v>44806</v>
+      </c>
+      <c r="I37" s="24"/>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B38">
+        <v>32</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D38" s="6">
+        <v>44805</v>
+      </c>
+      <c r="E38" s="6">
+        <v>44806</v>
+      </c>
+      <c r="I38" s="8"/>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B39">
+        <v>33</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D39" s="6">
+        <v>44805</v>
+      </c>
+      <c r="E39" s="6">
+        <v>44806</v>
+      </c>
+      <c r="I39" s="24"/>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C40" s="26"/>
+      <c r="D40" s="27"/>
+      <c r="E40" s="27"/>
+      <c r="F40" s="27"/>
+      <c r="G40" s="27"/>
+      <c r="H40" s="27"/>
+      <c r="I40" s="27"/>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C41" s="26"/>
+      <c r="D41" s="27"/>
+      <c r="E41" s="27"/>
+      <c r="F41" s="27"/>
+      <c r="G41" s="27"/>
+      <c r="H41" s="27"/>
+      <c r="I41" s="27"/>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C42" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
arreglo en HTML y CSS en productos
</commit_message>
<xml_diff>
--- a/Diagrama de Gatt.xlsx
+++ b/Diagrama de Gatt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\proyecto2022\practica2022NatalyAlvarez\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B835C444-3050-418A-B699-3EF1DDA89656}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95408173-D48C-46C9-8249-2C0900F90F27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{70482EC0-32A2-4E4F-95B6-32952FC475EF}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="41">
   <si>
     <t>Nombre de Actividad</t>
   </si>
@@ -153,6 +153,9 @@
   </si>
   <si>
     <t>Edición final de botones y orden burbuja para productos</t>
+  </si>
+  <si>
+    <t>Arreglo de errores en HTML,CSS de productos</t>
   </si>
 </sst>
 </file>
@@ -364,7 +367,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -409,8 +412,6 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Énfasis6" xfId="1" builtinId="49"/>
@@ -904,8 +905,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{166A0605-256A-4EC0-BEB8-5543620DF797}">
   <dimension ref="B5:O42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView tabSelected="1" topLeftCell="B19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1435,7 +1436,7 @@
       </c>
       <c r="I32" s="24"/>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B33">
         <v>27</v>
       </c>
@@ -1450,7 +1451,7 @@
       </c>
       <c r="I33" s="8"/>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B34">
         <v>28</v>
       </c>
@@ -1465,7 +1466,7 @@
       </c>
       <c r="I34" s="24"/>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B35">
         <v>29</v>
       </c>
@@ -1480,7 +1481,7 @@
       </c>
       <c r="I35" s="24"/>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B36">
         <v>30</v>
       </c>
@@ -1495,7 +1496,7 @@
       </c>
       <c r="I36" s="8"/>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B37">
         <v>31</v>
       </c>
@@ -1510,7 +1511,7 @@
       </c>
       <c r="I37" s="24"/>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B38">
         <v>32</v>
       </c>
@@ -1525,7 +1526,7 @@
       </c>
       <c r="I38" s="8"/>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B39">
         <v>33</v>
       </c>
@@ -1540,25 +1541,25 @@
       </c>
       <c r="I39" s="24"/>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C40" s="26"/>
-      <c r="D40" s="27"/>
-      <c r="E40" s="27"/>
-      <c r="F40" s="27"/>
-      <c r="G40" s="27"/>
-      <c r="H40" s="27"/>
-      <c r="I40" s="27"/>
-    </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C41" s="26"/>
-      <c r="D41" s="27"/>
-      <c r="E41" s="27"/>
-      <c r="F41" s="27"/>
-      <c r="G41" s="27"/>
-      <c r="H41" s="27"/>
-      <c r="I41" s="27"/>
-    </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B40">
+        <v>34</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D40" s="6">
+        <v>44806</v>
+      </c>
+      <c r="E40" s="6">
+        <v>44806</v>
+      </c>
+      <c r="J40" s="8"/>
+    </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C41" s="1"/>
+    </row>
+    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C42" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
documento de fase 02 en PDF y ordenado
</commit_message>
<xml_diff>
--- a/Diagrama de Gatt.xlsx
+++ b/Diagrama de Gatt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\proyecto2022\practica2022NatalyAlvarez\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95408173-D48C-46C9-8249-2C0900F90F27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87E520A1-BC29-4513-9DC1-9D9388914619}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{70482EC0-32A2-4E4F-95B6-32952FC475EF}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="42">
   <si>
     <t>Nombre de Actividad</t>
   </si>
@@ -156,13 +156,16 @@
   </si>
   <si>
     <t>Arreglo de errores en HTML,CSS de productos</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -217,8 +220,16 @@
       <name val="Calibri Light"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -242,8 +253,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -274,17 +291,6 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="0" tint="-0.24994659260841701"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0" tint="-0.24994659260841701"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -362,21 +368,86 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="16" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -386,22 +457,20 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -409,7 +478,62 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -449,9 +573,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>57149</xdr:colOff>
+      <xdr:colOff>103238</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>85724</xdr:rowOff>
+      <xdr:rowOff>116450</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2047875" cy="962025"/>
     <xdr:pic>
@@ -474,7 +598,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11439524" y="466724"/>
+          <a:off x="11840496" y="1038224"/>
           <a:ext cx="2047875" cy="962025"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -486,16 +610,16 @@
   </xdr:oneCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>41672</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:rowOff>138266</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>19386</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>725201</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>57283</xdr:rowOff>
+      <xdr:rowOff>79230</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -517,8 +641,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11325225" y="5200650"/>
-          <a:ext cx="2353011" cy="952633"/>
+          <a:off x="11778930" y="5668911"/>
+          <a:ext cx="2219819" cy="862738"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -903,668 +1027,788 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{166A0605-256A-4EC0-BEB8-5543620DF797}">
-  <dimension ref="B5:O42"/>
+  <dimension ref="A5:O43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="57" zoomScaleNormal="57" workbookViewId="0">
+      <selection activeCell="T34" sqref="T34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="18.140625" customWidth="1"/>
+    <col min="2" max="2" width="5.7109375" customWidth="1"/>
     <col min="3" max="3" width="81.5703125" customWidth="1"/>
     <col min="4" max="5" width="15" customWidth="1"/>
-    <col min="6" max="12" width="5.42578125" customWidth="1"/>
+    <col min="6" max="11" width="5.42578125" customWidth="1"/>
+    <col min="12" max="12" width="7.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C5" s="4" t="s">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B5" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="19" t="s">
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="N5" s="20"/>
-      <c r="O5" s="21"/>
-    </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C6" s="17"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="9" t="s">
+      <c r="N5" s="13"/>
+      <c r="O5" s="14"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="19"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="44"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="G6" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="H6" s="9" t="s">
+      <c r="H6" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="I6" s="9" t="s">
+      <c r="I6" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="J6" s="9" t="s">
+      <c r="J6" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="K6" s="9" t="s">
+      <c r="K6" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="L6" s="9" t="s">
+      <c r="L6" s="47" t="s">
         <v>36</v>
       </c>
-      <c r="M6" s="12"/>
-      <c r="O6" s="13"/>
-    </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B7">
+      <c r="M6" s="7"/>
+      <c r="O6" s="8"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B7" s="28">
         <v>1</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="24">
         <v>44774</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="24">
         <v>44780</v>
       </c>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9" t="s">
+      <c r="F7" s="4"/>
+      <c r="G7" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="H7" s="22"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="9"/>
-      <c r="L7" s="9"/>
-      <c r="M7" s="12"/>
-      <c r="O7" s="13"/>
-    </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B8">
+      <c r="H7" s="15"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="7"/>
+      <c r="O7" s="8"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B8" s="26">
         <v>2</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="24">
         <v>44775</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="24">
         <v>44780</v>
       </c>
-      <c r="H8" s="23"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="M8" s="12"/>
-      <c r="O8" s="13"/>
-    </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B9">
+      <c r="H8" s="16"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="M8" s="7"/>
+      <c r="O8" s="8"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B9" s="26">
         <v>3</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="24">
         <v>44775</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="24">
         <v>44780</v>
       </c>
-      <c r="I9" s="8"/>
-      <c r="M9" s="12"/>
-      <c r="O9" s="13"/>
-    </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B10">
+      <c r="I9" s="3"/>
+      <c r="M9" s="7"/>
+      <c r="O9" s="8"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B10" s="26">
         <v>4</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="24">
         <v>44776</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="24">
         <v>44780</v>
       </c>
-      <c r="J10" s="24"/>
-      <c r="M10" s="12"/>
-      <c r="O10" s="13"/>
-    </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B11">
+      <c r="J10" s="17"/>
+      <c r="M10" s="7"/>
+      <c r="O10" s="8"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B11" s="26">
         <v>5</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="24">
         <v>44777</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="24">
         <v>44780</v>
       </c>
-      <c r="J11" s="8"/>
-      <c r="K11" s="10"/>
-      <c r="M11" s="14"/>
-      <c r="N11" s="15"/>
-      <c r="O11" s="16"/>
-    </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B12">
+      <c r="J11" s="3"/>
+      <c r="K11" s="5"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="10"/>
+      <c r="O11" s="11"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B12" s="26">
         <v>6</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="24">
         <v>44778</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="24">
         <v>44780</v>
       </c>
-      <c r="F12" s="11"/>
-      <c r="K12" s="24"/>
-    </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B13">
+      <c r="F12" s="6"/>
+      <c r="K12" s="17"/>
+      <c r="M12" s="29"/>
+      <c r="N12" s="29"/>
+      <c r="O12" s="30"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B13" s="26">
         <v>7</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="24">
         <v>44778</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="24">
         <v>44780</v>
       </c>
-      <c r="F13" s="11"/>
-      <c r="K13" s="8"/>
-    </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B14">
+      <c r="F13" s="6"/>
+      <c r="K13" s="3"/>
+      <c r="M13" s="19"/>
+      <c r="N13" s="19"/>
+      <c r="O13" s="8"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B14" s="26">
         <v>8</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="6">
+      <c r="D14" s="24">
         <v>44778</v>
       </c>
-      <c r="E14" s="6">
+      <c r="E14" s="24">
         <v>44780</v>
       </c>
-      <c r="F14" s="11"/>
-      <c r="K14" s="24"/>
-    </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B15">
+      <c r="F14" s="6"/>
+      <c r="K14" s="17"/>
+      <c r="M14" s="19"/>
+      <c r="N14" s="19"/>
+      <c r="O14" s="8"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B15" s="26">
         <v>9</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="6">
+      <c r="D15" s="24">
         <v>44781</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E15" s="24">
         <v>44787</v>
       </c>
-      <c r="G15" s="11"/>
-      <c r="H15" s="8"/>
-    </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B16">
+      <c r="G15" s="6"/>
+      <c r="H15" s="3"/>
+      <c r="M15" s="19"/>
+      <c r="N15" s="19"/>
+      <c r="O15" s="8"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B16" s="26">
         <v>10</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="6">
+      <c r="D16" s="24">
         <v>44782</v>
       </c>
-      <c r="E16" s="6">
+      <c r="E16" s="24">
         <v>44787</v>
       </c>
-      <c r="F16" s="11"/>
-      <c r="H16" s="24"/>
-      <c r="J16" s="24"/>
+      <c r="F16" s="6"/>
+      <c r="H16" s="17"/>
+      <c r="J16" s="17"/>
+      <c r="M16" s="19"/>
+      <c r="N16" s="19"/>
+      <c r="O16" s="8"/>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B17">
+      <c r="B17" s="26">
         <v>11</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="D17" s="6">
+      <c r="D17" s="24">
         <v>44782</v>
       </c>
-      <c r="E17" s="6">
+      <c r="E17" s="24">
         <v>44787</v>
       </c>
-      <c r="F17" s="11"/>
-      <c r="H17" s="8"/>
-      <c r="J17" s="8"/>
+      <c r="F17" s="6"/>
+      <c r="H17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="M17" s="19"/>
+      <c r="N17" s="19"/>
+      <c r="O17" s="8"/>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B18">
+      <c r="B18" s="26">
         <v>12</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="6">
+      <c r="D18" s="24">
         <v>44783</v>
       </c>
-      <c r="E18" s="6">
+      <c r="E18" s="24">
         <v>44787</v>
       </c>
-      <c r="F18" s="11"/>
-      <c r="J18" s="24"/>
+      <c r="F18" s="6"/>
+      <c r="J18" s="17"/>
+      <c r="M18" s="19"/>
+      <c r="N18" s="19"/>
+      <c r="O18" s="8"/>
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B19">
+      <c r="B19" s="26">
         <v>13</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="D19" s="6">
+      <c r="D19" s="24">
         <v>44789</v>
       </c>
-      <c r="E19" s="6">
+      <c r="E19" s="24">
         <v>44792</v>
       </c>
-      <c r="F19" s="11"/>
-      <c r="H19" s="8"/>
+      <c r="F19" s="6"/>
+      <c r="H19" s="3"/>
+      <c r="M19" s="19"/>
+      <c r="N19" s="19"/>
+      <c r="O19" s="8"/>
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B20">
+      <c r="B20" s="26">
         <v>14</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="D20" s="6">
+      <c r="D20" s="24">
         <v>44791</v>
       </c>
-      <c r="E20" s="6">
+      <c r="E20" s="24">
         <v>44792</v>
       </c>
-      <c r="F20" s="11"/>
-      <c r="J20" s="8"/>
+      <c r="F20" s="6"/>
+      <c r="J20" s="3"/>
+      <c r="M20" s="19"/>
+      <c r="N20" s="19"/>
+      <c r="O20" s="8"/>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B21">
+      <c r="B21" s="26">
         <v>15</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="D21" s="6">
+      <c r="D21" s="24">
         <v>44791</v>
       </c>
-      <c r="E21" s="6">
+      <c r="E21" s="24">
         <v>44792</v>
       </c>
-      <c r="F21" s="11"/>
-      <c r="J21" s="24"/>
+      <c r="F21" s="6"/>
+      <c r="J21" s="17"/>
+      <c r="M21" s="19"/>
+      <c r="N21" s="19"/>
+      <c r="O21" s="8"/>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B22">
+      <c r="B22" s="26">
         <v>16</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="D22" s="6">
+      <c r="D22" s="24">
         <v>44792</v>
       </c>
-      <c r="E22" s="6">
+      <c r="E22" s="24">
         <v>44792</v>
       </c>
-      <c r="F22" s="11"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="8"/>
-      <c r="K22" s="8"/>
+      <c r="F22" s="6"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="M22" s="19"/>
+      <c r="N22" s="19"/>
+      <c r="O22" s="8"/>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B23">
+      <c r="B23" s="26">
         <v>17</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="D23" s="6">
+      <c r="D23" s="24">
         <v>44795</v>
       </c>
-      <c r="E23" s="6">
+      <c r="E23" s="24">
         <v>44799</v>
       </c>
-      <c r="F23" s="8"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="H23" s="40"/>
+      <c r="I23" s="40"/>
+      <c r="J23" s="40"/>
+      <c r="K23" s="40"/>
+      <c r="M23" s="19"/>
+      <c r="N23" s="19"/>
+      <c r="O23" s="8"/>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B24">
+      <c r="B24" s="26">
         <v>18</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="D24" s="6">
+      <c r="D24" s="24">
         <v>44797</v>
       </c>
-      <c r="E24" s="6">
+      <c r="E24" s="24">
         <v>44799</v>
       </c>
-      <c r="G24" s="24"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
-      <c r="K24" s="3"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="40"/>
+      <c r="I24" s="40"/>
+      <c r="J24" s="40"/>
+      <c r="K24" s="40"/>
+      <c r="M24" s="19"/>
+      <c r="N24" s="19"/>
+      <c r="O24" s="8"/>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B25">
+      <c r="B25" s="26">
         <v>19</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="D25" s="6">
+      <c r="D25" s="24">
         <v>44798</v>
       </c>
-      <c r="E25" s="6">
+      <c r="E25" s="24">
         <v>44799</v>
       </c>
-      <c r="F25" s="11"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
-      <c r="K25" s="3"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="41"/>
+      <c r="I25" s="36"/>
+      <c r="J25" s="36"/>
+      <c r="K25" s="36"/>
+      <c r="L25" s="34"/>
+      <c r="M25" s="19"/>
+      <c r="N25" s="19"/>
+      <c r="O25" s="8"/>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B26">
+      <c r="B26" s="26">
         <v>20</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="D26" s="6">
+      <c r="D26" s="24">
         <v>44802</v>
       </c>
-      <c r="E26" s="6">
+      <c r="E26" s="24">
         <v>44806</v>
       </c>
-      <c r="F26" s="11"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="24"/>
-      <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
-      <c r="K26" s="3"/>
+      <c r="F26" s="38"/>
+      <c r="G26" s="38"/>
+      <c r="H26" s="17"/>
+      <c r="I26" s="36"/>
+      <c r="J26" s="36"/>
+      <c r="K26" s="36"/>
+      <c r="L26" s="35"/>
+      <c r="M26" s="19"/>
+      <c r="N26" s="19"/>
+      <c r="O26" s="8"/>
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B27">
+      <c r="B27" s="26">
         <v>21</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C27" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="D27" s="6">
+      <c r="D27" s="24">
         <v>44802</v>
       </c>
-      <c r="E27" s="6">
+      <c r="E27" s="24">
         <v>44806</v>
       </c>
-      <c r="F27" s="11"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="8"/>
-      <c r="K27" s="3"/>
+      <c r="F27" s="38"/>
+      <c r="G27" s="38"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="36"/>
+      <c r="J27" s="36"/>
+      <c r="K27" s="36"/>
+      <c r="L27" s="35"/>
+      <c r="M27" s="19"/>
+      <c r="N27" s="19"/>
+      <c r="O27" s="8"/>
     </row>
     <row r="28" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B28">
+      <c r="B28" s="26">
         <v>22</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="D28" s="6">
+      <c r="D28" s="24">
         <v>44802</v>
       </c>
-      <c r="E28" s="6">
+      <c r="E28" s="24">
         <v>44806</v>
       </c>
-      <c r="F28" s="11"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
-      <c r="I28" s="24"/>
-      <c r="K28" s="3"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="37"/>
+      <c r="I28" s="17"/>
+      <c r="K28" s="39"/>
+      <c r="L28" s="39"/>
+      <c r="M28" s="19"/>
+      <c r="N28" s="19"/>
+      <c r="O28" s="8"/>
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B29">
+      <c r="B29" s="26">
         <v>23</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C29" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="D29" s="6">
+      <c r="D29" s="24">
         <v>44802</v>
       </c>
-      <c r="E29" s="6">
+      <c r="E29" s="24">
         <v>44806</v>
       </c>
-      <c r="F29" s="11"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="8"/>
-      <c r="K29" s="3"/>
+      <c r="F29" s="38"/>
+      <c r="H29" s="36"/>
+      <c r="I29" s="3"/>
+      <c r="K29" s="39"/>
+      <c r="L29" s="39"/>
+      <c r="M29" s="19"/>
+      <c r="N29" s="19"/>
+      <c r="O29" s="8"/>
     </row>
     <row r="30" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B30">
+      <c r="B30" s="26">
         <v>24</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C30" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="D30" s="6">
+      <c r="D30" s="24">
         <v>44805</v>
       </c>
-      <c r="E30" s="6">
+      <c r="E30" s="24">
         <v>44806</v>
       </c>
-      <c r="F30" s="6"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="24"/>
-      <c r="K30" s="3"/>
-      <c r="L30" s="3"/>
-      <c r="M30" s="25" t="s">
+      <c r="F30" s="38"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="36"/>
+      <c r="I30" s="17"/>
+      <c r="K30" s="39"/>
+      <c r="L30" s="39"/>
+      <c r="M30" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="N30" s="25"/>
-      <c r="O30" s="25"/>
+      <c r="N30" s="31"/>
+      <c r="O30" s="32"/>
     </row>
     <row r="31" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B31">
+      <c r="B31" s="26">
         <v>25</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C31" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="D31" s="6">
+      <c r="D31" s="24">
         <v>44805</v>
       </c>
-      <c r="E31" s="6">
+      <c r="E31" s="24">
         <v>44806</v>
       </c>
-      <c r="I31" s="8"/>
+      <c r="F31" s="38"/>
+      <c r="H31" s="36"/>
+      <c r="I31" s="3"/>
+      <c r="K31" s="39"/>
+      <c r="L31" s="39"/>
+      <c r="M31" s="7"/>
+      <c r="N31" s="19"/>
+      <c r="O31" s="8"/>
     </row>
     <row r="32" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B32">
+      <c r="B32" s="26">
         <v>26</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C32" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="D32" s="6">
+      <c r="D32" s="49">
         <v>44805</v>
       </c>
-      <c r="E32" s="6">
+      <c r="E32" s="49">
         <v>44806</v>
       </c>
-      <c r="I32" s="24"/>
-    </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B33">
+      <c r="F32" s="38"/>
+      <c r="I32" s="17"/>
+      <c r="K32" s="39"/>
+      <c r="L32" s="39"/>
+      <c r="M32" s="7"/>
+      <c r="N32" s="19"/>
+      <c r="O32" s="8"/>
+    </row>
+    <row r="33" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B33" s="26">
         <v>27</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C33" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="D33" s="6">
+      <c r="D33" s="24">
         <v>44805</v>
       </c>
-      <c r="E33" s="6">
+      <c r="E33" s="24">
         <v>44806</v>
       </c>
-      <c r="I33" s="8"/>
-    </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B34">
+      <c r="I33" s="3"/>
+      <c r="M33" s="7"/>
+      <c r="N33" s="19"/>
+      <c r="O33" s="8"/>
+    </row>
+    <row r="34" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B34" s="26">
         <v>28</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C34" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="D34" s="6">
+      <c r="D34" s="24">
         <v>44805</v>
       </c>
-      <c r="E34" s="6">
+      <c r="E34" s="24">
         <v>44806</v>
       </c>
-      <c r="I34" s="24"/>
-    </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B35">
+      <c r="I34" s="17"/>
+      <c r="M34" s="7"/>
+      <c r="N34" s="19"/>
+      <c r="O34" s="8"/>
+    </row>
+    <row r="35" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B35" s="26">
         <v>29</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C35" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="D35" s="6">
+      <c r="D35" s="24">
         <v>44805</v>
       </c>
-      <c r="E35" s="6">
+      <c r="E35" s="24">
         <v>44806</v>
       </c>
-      <c r="I35" s="24"/>
-    </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B36">
+      <c r="I35" s="17"/>
+      <c r="M35" s="7"/>
+      <c r="N35" s="19"/>
+      <c r="O35" s="8"/>
+    </row>
+    <row r="36" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B36" s="26">
         <v>30</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C36" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="D36" s="6">
+      <c r="D36" s="24">
         <v>44805</v>
       </c>
-      <c r="E36" s="6">
+      <c r="E36" s="24">
         <v>44806</v>
       </c>
-      <c r="I36" s="8"/>
-    </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B37">
+      <c r="I36" s="3"/>
+      <c r="M36" s="9"/>
+      <c r="N36" s="10"/>
+      <c r="O36" s="11"/>
+    </row>
+    <row r="37" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B37" s="26">
         <v>31</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C37" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="D37" s="6">
+      <c r="D37" s="24">
         <v>44805</v>
       </c>
-      <c r="E37" s="6">
+      <c r="E37" s="24">
         <v>44806</v>
       </c>
-      <c r="I37" s="24"/>
-    </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B38">
+      <c r="I37" s="17"/>
+      <c r="M37" s="19"/>
+      <c r="N37" s="19"/>
+      <c r="O37" s="8"/>
+    </row>
+    <row r="38" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B38" s="26">
         <v>32</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C38" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="D38" s="6">
+      <c r="D38" s="22">
         <v>44805</v>
       </c>
-      <c r="E38" s="6">
+      <c r="E38" s="22">
         <v>44806</v>
       </c>
-      <c r="I38" s="8"/>
-    </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B39">
+      <c r="I38" s="3"/>
+      <c r="M38" s="19"/>
+      <c r="N38" s="19"/>
+      <c r="O38" s="8"/>
+    </row>
+    <row r="39" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B39" s="26">
         <v>33</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C39" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="D39" s="6">
+      <c r="D39" s="21">
         <v>44805</v>
       </c>
-      <c r="E39" s="6">
+      <c r="E39" s="21">
         <v>44806</v>
       </c>
-      <c r="I39" s="24"/>
-    </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B40">
+      <c r="I39" s="17"/>
+      <c r="M39" s="19"/>
+      <c r="N39" s="19"/>
+      <c r="O39" s="8"/>
+    </row>
+    <row r="40" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B40" s="26">
         <v>34</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C40" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="D40" s="6">
+      <c r="D40" s="24">
         <v>44806</v>
       </c>
-      <c r="E40" s="6">
+      <c r="E40" s="24">
         <v>44806</v>
       </c>
-      <c r="J40" s="8"/>
-    </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C41" s="1"/>
-    </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C42" s="1"/>
+      <c r="F40" s="10"/>
+      <c r="G40" s="10"/>
+      <c r="H40" s="10"/>
+      <c r="I40" s="10"/>
+      <c r="J40" s="33"/>
+      <c r="K40" s="10"/>
+      <c r="L40" s="10"/>
+      <c r="M40" s="10"/>
+      <c r="N40" s="10"/>
+      <c r="O40" s="11"/>
+    </row>
+    <row r="41" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B41" s="43"/>
+      <c r="C41" s="43"/>
+    </row>
+    <row r="42" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B42" s="42"/>
+      <c r="C42" s="42"/>
+    </row>
+    <row r="43" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B43" s="42"/>
+      <c r="C43" s="42"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="6">
+    <mergeCell ref="B41:C43"/>
     <mergeCell ref="M30:O30"/>
+    <mergeCell ref="F26:G28"/>
+    <mergeCell ref="F29:F32"/>
+    <mergeCell ref="H28:H31"/>
+    <mergeCell ref="I25:K27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>